<commit_message>
1.protobuf 生成ts数据结构以及parser 2.fix 数据库存储设置 kv模式下没有value(value都设置成unique导致没有value) 3.fix relay 在global => relay => user => relay => global死循环 4.DataTypeHelper ToString bug, 引号多了
Former-commit-id: e5b390b6723d24ae14f4dd05eb6e68a9ffc01b01
</commit_message>
<xml_diff>
--- a/service/TestService/config/xlsx/公共参数.xlsx
+++ b/service/TestService/config/xlsx/公共参数.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Development\CrystalNetGithub\CrystalNet\service\TestService\config\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A4EC6FD-8F02-4510-B2EC-C1E6086342DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E03E975-AC6E-48BF-B9A6-9946B244C626}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="50">
   <si>
     <t>C|S</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -216,6 +216,14 @@
   </si>
   <si>
     <t>一周开始, 若是过往是从0(星期天)开始, 国内是从1(星期一)开始</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CREATE_LIBRARY_NEED_INVITE_CODE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>创建图书馆是否需要邀请码</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -548,10 +556,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F20"/>
+  <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -836,6 +844,20 @@
         <v>47</v>
       </c>
     </row>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>48</v>
+      </c>
+      <c r="C21">
+        <v>0</v>
+      </c>
+      <c r="D21">
+        <v>0</v>
+      </c>
+      <c r="F21" t="s">
+        <v>49</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
1. log IsEnable优化 2. epoll/iocp session fix recvBuffer 在ParsingPacket失败后没有Erase(node)导致节点重复释放报错 3.优化逻辑
Former-commit-id: 77cb03e31daf51f372172e1137dba80ca510852d
</commit_message>
<xml_diff>
--- a/service/TestService/config/xlsx/公共参数.xlsx
+++ b/service/TestService/config/xlsx/公共参数.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Development\CrystalNetGithub\CrystalNet\service\TestService\config\xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workplace\mine\CrystalNet\CrystalNet\service\TestService\config\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1F98F02-E1BF-4CD1-82EB-BDD6FEF3B8A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AF40438-F1F4-4053-AB80-77B8E676359E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30612" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="公共参数|Common" sheetId="1" r:id="rId1"/>
@@ -231,7 +231,7 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>最大图片大小2MB</t>
+    <t>最大图片大小76KB</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -567,7 +567,7 @@
   <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -871,10 +871,10 @@
         <v>50</v>
       </c>
       <c r="C22">
-        <v>2097152</v>
+        <v>77824</v>
       </c>
       <c r="D22">
-        <v>2097152</v>
+        <v>77824</v>
       </c>
       <c r="F22" t="s">
         <v>51</v>

</xml_diff>